<commit_message>
tests: df_tables_config_options: input: before tables_config:
</commit_message>
<xml_diff>
--- a/src/yarm/tests_data/test_create_tables/orders.xlsx
+++ b/src/yarm/tests_data/test_create_tables/orders.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" state="visible" r:id="rId2"/>
@@ -51,6 +51,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,8 +111,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -138,47 +143,47 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="211" zoomScaleNormal="211" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="211" zoomScaleNormal="211" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>38261</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>333</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>1001</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>38262</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>333</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1"/>
+      <c r="B4" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -198,49 +203,49 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="211" zoomScaleNormal="211" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="211" zoomScaleNormal="211" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>1001</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>1001</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>